<commit_message>
End To End All Modules
</commit_message>
<xml_diff>
--- a/Team17_APINinjas_LMSHack/src/test/resources/LMSAPINinjaTestData.xlsx
+++ b/Team17_APINinjas_LMSHack/src/test/resources/LMSAPINinjaTestData.xlsx
@@ -4,19 +4,24 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="22950" windowHeight="9360" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="22950" windowHeight="9360" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="GetDeleteTestData-BatchJyo" sheetId="5" r:id="rId1"/>
     <sheet name="PostPutTestData-BatchJyo" sheetId="6" r:id="rId2"/>
     <sheet name="ETEPositiveTestData" sheetId="10" r:id="rId3"/>
+    <sheet name="PostUser" sheetId="11" r:id="rId4"/>
+    <sheet name="PutUser" sheetId="12" r:id="rId5"/>
+    <sheet name="PutLoginStatus" sheetId="13" r:id="rId6"/>
+    <sheet name="PositiveTestDataPrgmBatchStatus" sheetId="14" r:id="rId7"/>
+    <sheet name="PutProgramBatchStatus" sheetId="15" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="157">
   <si>
     <t>TestCaseNumbers</t>
   </si>
@@ -234,12 +239,6 @@
     <t>ffg16jhg55g5</t>
   </si>
   <si>
-    <t>8 4 6 8</t>
-  </si>
-  <si>
-    <t>1 6 5 5 5</t>
-  </si>
-  <si>
     <t>8&amp;^4$%6&amp;8</t>
   </si>
   <si>
@@ -325,13 +324,181 @@
   </si>
   <si>
     <t>Numpyninja@1</t>
+  </si>
+  <si>
+    <t>8 7 5 2</t>
+  </si>
+  <si>
+    <t>1 6 4 4 8</t>
+  </si>
+  <si>
+    <t>updateRoleID</t>
+  </si>
+  <si>
+    <t>updateRoleStatus</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>R03</t>
+  </si>
+  <si>
+    <t>userId</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>timeZone</t>
+  </si>
+  <si>
+    <t>visaStatus</t>
+  </si>
+  <si>
+    <t>middleName</t>
+  </si>
+  <si>
+    <t>linkedinUrl</t>
+  </si>
+  <si>
+    <t>eduUg</t>
+  </si>
+  <si>
+    <t>eduPg</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>userLogin.loginStatus</t>
+  </si>
+  <si>
+    <t>userLogin.password</t>
+  </si>
+  <si>
+    <t>userLogin.status</t>
+  </si>
+  <si>
+    <t>userLogin.userLoginEmail</t>
+  </si>
+  <si>
+    <t>userLogin.roleIds</t>
+  </si>
+  <si>
+    <t>userRoleMaps.userRoleStatus</t>
+  </si>
+  <si>
+    <t>userRoleMaps.roleId</t>
+  </si>
+  <si>
+    <t>expectedResponseCode</t>
+  </si>
+  <si>
+    <t>APINinjas</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>PST</t>
+  </si>
+  <si>
+    <t>Canada-Citizen</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/meena/</t>
+  </si>
+  <si>
+    <t>BSC</t>
+  </si>
+  <si>
+    <t>MSC</t>
+  </si>
+  <si>
+    <t>ROLE_STAFF</t>
+  </si>
+  <si>
+    <t>Seattle</t>
+  </si>
+  <si>
+    <t>hack023</t>
+  </si>
+  <si>
+    <t>R02</t>
+  </si>
+  <si>
+    <t>Create User- Mandatory fields</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>ROLE_STUDENT</t>
+  </si>
+  <si>
+    <t>R01</t>
+  </si>
+  <si>
+    <t>4156169xxx</t>
+  </si>
+  <si>
+    <t>APIemailxxx@gmail.com</t>
+  </si>
+  <si>
+    <t>4356169xxx</t>
+  </si>
+  <si>
+    <t>Ninjasemailxxx@gmail.com</t>
+  </si>
+  <si>
+    <t>4456169xxx</t>
+  </si>
+  <si>
+    <t>APINinjasmyemailxxx@gmail.com</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>UserID</t>
+  </si>
+  <si>
+    <t>RoleID</t>
+  </si>
+  <si>
+    <t>U404</t>
+  </si>
+  <si>
+    <t>roleId</t>
+  </si>
+  <si>
+    <t>batchId</t>
+  </si>
+  <si>
+    <t>userRoleProgramBatchStatus</t>
+  </si>
+  <si>
+    <t>Update User- Mandatory fields</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -351,6 +518,28 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -450,10 +639,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -560,8 +753,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -857,7 +1080,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -885,13 +1108,13 @@
         <v>53</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F1" s="16" t="s">
         <v>54</v>
       </c>
       <c r="G1" s="25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30.75" thickBot="1">
@@ -899,10 +1122,10 @@
         <v>68</v>
       </c>
       <c r="B2" s="18">
-        <v>8468</v>
+        <v>8887</v>
       </c>
       <c r="C2" s="18">
-        <v>16555</v>
+        <v>16730</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>69</v>
@@ -917,7 +1140,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1">
+    <row r="3" spans="1:7" ht="30.75" thickBot="1">
       <c r="A3" s="17" t="s">
         <v>55</v>
       </c>
@@ -940,7 +1163,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="29.25" thickBot="1">
+    <row r="4" spans="1:7" ht="43.5" thickBot="1">
       <c r="A4" s="19" t="s">
         <v>57</v>
       </c>
@@ -963,7 +1186,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="29.25" thickBot="1">
+    <row r="5" spans="1:7" ht="43.5" thickBot="1">
       <c r="A5" s="19" t="s">
         <v>59</v>
       </c>
@@ -986,7 +1209,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="57.75" thickBot="1">
+    <row r="6" spans="1:7" ht="86.25" thickBot="1">
       <c r="A6" s="19" t="s">
         <v>61</v>
       </c>
@@ -997,7 +1220,7 @@
         <v>62</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E6" s="20">
         <v>401</v>
@@ -1009,14 +1232,14 @@
         <v>401</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="43.5" thickBot="1">
+    <row r="7" spans="1:7" ht="57.75" thickBot="1">
       <c r="A7" s="19" t="s">
         <v>63</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="18"/>
       <c r="D7" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E7" s="20">
         <v>405</v>
@@ -1028,18 +1251,18 @@
         <v>405</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="72" thickBot="1">
+    <row r="8" spans="1:7" ht="86.25" thickBot="1">
       <c r="A8" s="19" t="s">
         <v>64</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E8" s="22">
         <v>401</v>
@@ -1051,15 +1274,15 @@
         <v>401</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="29.25" thickBot="1">
+    <row r="9" spans="1:7" ht="43.5" thickBot="1">
       <c r="A9" s="22" t="s">
         <v>65</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="23">
@@ -1081,8 +1304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1105,7 +1328,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="30.75" thickBot="1">
       <c r="A1" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>2</v>
@@ -1152,7 +1375,7 @@
         <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D2" s="3">
         <v>10</v>
@@ -1161,13 +1384,13 @@
         <v>15</v>
       </c>
       <c r="F2" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I2" s="3">
         <v>18</v>
@@ -1176,10 +1399,10 @@
         <v>15</v>
       </c>
       <c r="K2" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="L2" s="7">
-        <v>201</v>
+        <v>400</v>
       </c>
       <c r="M2" s="7">
         <v>500</v>
@@ -1193,7 +1416,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D3" s="3">
         <v>10</v>
@@ -1202,13 +1425,13 @@
         <v>15</v>
       </c>
       <c r="F3" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I3" s="3">
         <v>18</v>
@@ -1217,7 +1440,7 @@
         <v>15</v>
       </c>
       <c r="K3" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="L3" s="7">
         <v>400</v>
@@ -1228,11 +1451,11 @@
     </row>
     <row r="4" spans="1:13" s="29" customFormat="1" ht="30.75" thickBot="1">
       <c r="A4" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B4" s="27"/>
       <c r="C4" s="27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D4" s="27">
         <v>10</v>
@@ -1240,12 +1463,12 @@
       <c r="E4" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="27">
-        <v>16766</v>
+      <c r="F4" s="3">
+        <v>16448</v>
       </c>
       <c r="G4" s="27"/>
       <c r="H4" s="27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I4" s="27">
         <v>18</v>
@@ -1253,8 +1476,8 @@
       <c r="J4" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="27">
-        <v>16766</v>
+      <c r="K4" s="3">
+        <v>16448</v>
       </c>
       <c r="L4" s="28">
         <v>201</v>
@@ -1265,13 +1488,13 @@
     </row>
     <row r="5" spans="1:13" ht="30.75" thickBot="1">
       <c r="A5" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D5" s="3">
         <v>10</v>
@@ -1280,13 +1503,13 @@
         <v>15</v>
       </c>
       <c r="F5" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I5" s="3">
         <v>18</v>
@@ -1295,7 +1518,7 @@
         <v>15</v>
       </c>
       <c r="K5" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="L5" s="7">
         <v>400</v>
@@ -1306,7 +1529,7 @@
     </row>
     <row r="6" spans="1:13" ht="30" thickBot="1">
       <c r="A6" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>14</v>
@@ -1337,27 +1560,27 @@
         <v>14</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="K7" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="L7" s="7">
         <v>400</v>
@@ -1374,27 +1597,27 @@
         <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D8" s="3">
         <v>10</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I8" s="3">
         <v>18</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="L8" s="7">
         <v>400</v>
@@ -1411,7 +1634,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D9" s="3">
         <v>10</v>
@@ -1424,7 +1647,7 @@
         <v>16</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I9" s="3">
         <v>18</v>
@@ -1457,7 +1680,7 @@
         <v>15</v>
       </c>
       <c r="F10" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>16</v>
@@ -1472,7 +1695,7 @@
         <v>15</v>
       </c>
       <c r="K10" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="L10" s="11">
         <v>400</v>
@@ -1496,7 +1719,7 @@
         <v>15</v>
       </c>
       <c r="F11" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>16</v>
@@ -1509,7 +1732,7 @@
         <v>15</v>
       </c>
       <c r="K11" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="L11" s="7">
         <v>400</v>
@@ -1535,7 +1758,7 @@
         <v>15</v>
       </c>
       <c r="F12" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>16</v>
@@ -1550,7 +1773,7 @@
         <v>15</v>
       </c>
       <c r="K12" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="L12" s="7">
         <v>400</v>
@@ -1567,7 +1790,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D13" s="3">
         <v>10</v>
@@ -1576,13 +1799,13 @@
         <v>15</v>
       </c>
       <c r="F13" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I13" s="3">
         <v>18</v>
@@ -1591,7 +1814,7 @@
         <v>15</v>
       </c>
       <c r="K13" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="L13" s="7">
         <v>400</v>
@@ -1608,7 +1831,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D14" s="3">
         <v>0</v>
@@ -1617,13 +1840,13 @@
         <v>15</v>
       </c>
       <c r="F14" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I14" s="3">
         <v>0</v>
@@ -1632,7 +1855,7 @@
         <v>15</v>
       </c>
       <c r="K14" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="L14" s="7">
         <v>400</v>
@@ -1649,7 +1872,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D15" s="3">
         <v>-10</v>
@@ -1658,13 +1881,13 @@
         <v>15</v>
       </c>
       <c r="F15" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I15" s="3">
         <v>-18</v>
@@ -1673,7 +1896,7 @@
         <v>15</v>
       </c>
       <c r="K15" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="L15" s="7">
         <v>400</v>
@@ -1690,7 +1913,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D16" s="3">
         <v>10</v>
@@ -1699,13 +1922,13 @@
         <v>32</v>
       </c>
       <c r="F16" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I16" s="3">
         <v>18</v>
@@ -1714,7 +1937,7 @@
         <v>32</v>
       </c>
       <c r="K16" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="L16" s="7">
         <v>400</v>
@@ -1731,7 +1954,7 @@
         <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D17" s="3">
         <v>10</v>
@@ -1740,13 +1963,13 @@
         <v>34</v>
       </c>
       <c r="F17" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I17" s="3">
         <v>18</v>
@@ -1755,7 +1978,7 @@
         <v>34</v>
       </c>
       <c r="K17" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="L17" s="7">
         <v>400</v>
@@ -1772,7 +1995,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D18" s="3">
         <v>10</v>
@@ -1781,13 +2004,13 @@
         <v>36</v>
       </c>
       <c r="F18" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I18" s="3">
         <v>18</v>
@@ -1796,7 +2019,7 @@
         <v>36</v>
       </c>
       <c r="K18" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="L18" s="7">
         <v>400</v>
@@ -1813,7 +2036,7 @@
         <v>14</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D19" s="3">
         <v>10</v>
@@ -1822,13 +2045,13 @@
         <v>234567</v>
       </c>
       <c r="F19" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I19" s="3">
         <v>18</v>
@@ -1837,7 +2060,7 @@
         <v>234567</v>
       </c>
       <c r="K19" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="L19" s="7">
         <v>400</v>
@@ -1854,7 +2077,7 @@
         <v>14</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D20" s="3">
         <v>10</v>
@@ -1863,13 +2086,13 @@
         <v>39</v>
       </c>
       <c r="F20" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I20" s="3">
         <v>18</v>
@@ -1878,7 +2101,7 @@
         <v>39</v>
       </c>
       <c r="K20" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="L20" s="7">
         <v>400</v>
@@ -1895,7 +2118,7 @@
         <v>14</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D21" s="3">
         <v>10</v>
@@ -1910,7 +2133,7 @@
         <v>16</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I21" s="3">
         <v>18</v>
@@ -1936,7 +2159,7 @@
         <v>14</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D22" s="3">
         <v>10</v>
@@ -1951,7 +2174,7 @@
         <v>16</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I22" s="3">
         <v>18</v>
@@ -1977,7 +2200,7 @@
         <v>14</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D23" s="3">
         <v>10</v>
@@ -1986,13 +2209,13 @@
         <v>15</v>
       </c>
       <c r="F23" s="3">
-        <v>-16766</v>
+        <v>-16448</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I23" s="3">
         <v>18</v>
@@ -2001,7 +2224,7 @@
         <v>15</v>
       </c>
       <c r="K23" s="3">
-        <v>-16766</v>
+        <v>-16448</v>
       </c>
       <c r="L23" s="7">
         <v>400</v>
@@ -2018,7 +2241,7 @@
         <v>44</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D24" s="3">
         <v>10</v>
@@ -2027,13 +2250,13 @@
         <v>15</v>
       </c>
       <c r="F24" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>44</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I24" s="3">
         <v>18</v>
@@ -2042,7 +2265,7 @@
         <v>15</v>
       </c>
       <c r="K24" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="L24" s="7">
         <v>400</v>
@@ -2059,7 +2282,7 @@
         <v>2345678</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D25" s="3">
         <v>10</v>
@@ -2068,13 +2291,13 @@
         <v>15</v>
       </c>
       <c r="F25" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="G25" s="3">
         <v>2345678</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I25" s="3">
         <v>18</v>
@@ -2083,7 +2306,7 @@
         <v>15</v>
       </c>
       <c r="K25" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="L25" s="7">
         <v>400</v>
@@ -2100,7 +2323,7 @@
         <v>47</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D26" s="3">
         <v>10</v>
@@ -2109,13 +2332,13 @@
         <v>15</v>
       </c>
       <c r="F26" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>48</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I26" s="3">
         <v>18</v>
@@ -2124,7 +2347,7 @@
         <v>15</v>
       </c>
       <c r="K26" s="3">
-        <v>16766</v>
+        <v>16448</v>
       </c>
       <c r="L26" s="7">
         <v>400</v>
@@ -2141,7 +2364,7 @@
         <v>14</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D27" s="3">
         <v>10</v>
@@ -2156,7 +2379,7 @@
         <v>16</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I27" s="3">
         <v>18</v>
@@ -2181,10 +2404,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2197,7 +2420,7 @@
     <col min="10" max="10" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="61.5" thickTop="1" thickBot="1">
+    <row r="1" spans="1:18" ht="61.5" thickTop="1" thickBot="1">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -2205,22 +2428,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E1" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="H1" s="30" t="s">
         <v>93</v>
-      </c>
-      <c r="G1" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="H1" s="30" t="s">
-        <v>95</v>
       </c>
       <c r="I1" s="30" t="s">
         <v>12</v>
@@ -2246,28 +2469,34 @@
       <c r="P1" s="31" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="45.75" thickBot="1">
+      <c r="Q1" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="R1" s="31" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="45.75" thickBot="1">
       <c r="A2" s="34" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B2" s="33" t="s">
         <v>50</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>15</v>
@@ -2295,6 +2524,550 @@
       </c>
       <c r="P2" s="32" t="s">
         <v>15</v>
+      </c>
+      <c r="Q2" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="R2" s="32" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:U2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:21" ht="60.75" thickBot="1">
+      <c r="A1" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="U1" s="36" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="75.75" thickBot="1">
+      <c r="A2" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="T2" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="U2" s="35">
+        <v>201</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="Q2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:U2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:21" ht="60.75" thickBot="1">
+      <c r="A1" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="U1" s="36" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="75.75" thickBot="1">
+      <c r="A2" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="35">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="Q2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:U2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:21" ht="60.75" thickBot="1">
+      <c r="A1" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="U1" s="36" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="75.75" thickBot="1">
+      <c r="A2" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="35">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="R2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="60.75" thickBot="1">
+      <c r="A1" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="43" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" s="43" t="s">
+        <v>151</v>
+      </c>
+      <c r="G1" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="45.75" thickBot="1">
+      <c r="A2" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="33">
+        <v>16652</v>
+      </c>
+      <c r="C2" s="33">
+        <v>8608</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="G2" s="34">
+        <v>200</v>
+      </c>
+      <c r="H2" s="34">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="45.75" thickBot="1">
+      <c r="A1" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>153</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" s="46" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" s="47" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A2" s="48" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Negative scenarios for user details
</commit_message>
<xml_diff>
--- a/Team17_APINinjas_LMSHack/src/test/resources/LMSAPINinjaTestData.xlsx
+++ b/Team17_APINinjas_LMSHack/src/test/resources/LMSAPINinjaTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Java\Team17_APINinjas\Team17_APINinjas_LMSHack\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446E051C-9601-4342-BBA4-1DFEEE77AD5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA0431E-0E72-4F19-A828-CB67CCA0F39F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PutLoginStatusNegative" sheetId="17" r:id="rId1"/>
@@ -22,15 +22,16 @@
     <sheet name="PutUser" sheetId="12" r:id="rId7"/>
     <sheet name="PutLoginStatus" sheetId="13" r:id="rId8"/>
     <sheet name="PutProgramBatchStatusNegative" sheetId="18" r:id="rId9"/>
-    <sheet name="PositiveTestDataPrgmBatchStatus" sheetId="14" r:id="rId10"/>
-    <sheet name="PutProgramBatchStatus" sheetId="15" r:id="rId11"/>
+    <sheet name="PutUserIdNegative" sheetId="19" r:id="rId10"/>
+    <sheet name="PositiveTestDataPrgmBatchStatus" sheetId="14" r:id="rId11"/>
+    <sheet name="PutProgramBatchStatus" sheetId="15" r:id="rId12"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="196">
   <si>
     <t>TestCaseNumbers</t>
   </si>
@@ -612,6 +613,12 @@
   </si>
   <si>
     <t>Update User- Unknown RoleprogrambatchStatus</t>
+  </si>
+  <si>
+    <t>U2361111</t>
+  </si>
+  <si>
+    <t>PSTXX</t>
   </si>
 </sst>
 </file>
@@ -766,7 +773,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -913,7 +920,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1393,6 +1399,173 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C869987-B931-453F-B22C-FCE8289E4B68}">
+  <dimension ref="A1:O3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="32.6328125" customWidth="1"/>
+    <col min="14" max="14" width="23.54296875" customWidth="1"/>
+    <col min="15" max="15" width="20.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="O1" s="36" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="73" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="N2" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="O2" s="49" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="73" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I3" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="N3" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="O3" s="49" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{5E8E8A38-A801-4B5A-BEEA-71DFDFC91883}"/>
+    <hyperlink ref="N2" r:id="rId2" xr:uid="{163E956C-A713-4F6B-8B33-E1A06D62B693}"/>
+    <hyperlink ref="I3" r:id="rId3" xr:uid="{FC1F64FF-340E-4724-B0D3-A76F91F4D6E2}"/>
+    <hyperlink ref="N3" r:id="rId4" xr:uid="{36D84669-5665-4E79-918C-0DA371968D14}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -1459,7 +1632,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -3476,7 +3649,7 @@
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3751,7 +3924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{592C7846-7F54-46C4-9F7C-BE63FE12C252}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
@@ -3786,7 +3959,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="51" t="s">
         <v>188</v>
       </c>
       <c r="B2" s="48" t="s">

</xml_diff>

<commit_message>
renaming the feature file tags
</commit_message>
<xml_diff>
--- a/Team17_APINinjas_LMSHack/src/test/resources/LMSAPINinjaTestData.xlsx
+++ b/Team17_APINinjas_LMSHack/src/test/resources/LMSAPINinjaTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="22950" windowHeight="9360" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="22950" windowHeight="9360" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GetDeleteTestData-BatchJyo" sheetId="5" r:id="rId1"/>
@@ -230,9 +230,6 @@
     <t>Deleted Ids,name</t>
   </si>
   <si>
-    <t>March24-ApINinjas-QA-QA1-013</t>
-  </si>
-  <si>
     <t>8b4rt6jhb8</t>
   </si>
   <si>
@@ -492,6 +489,9 @@
   </si>
   <si>
     <t>Update User- Mandatory fields</t>
+  </si>
+  <si>
+    <t>March24-Api Ninjas</t>
   </si>
 </sst>
 </file>
@@ -646,7 +646,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -715,9 +715,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1080,7 +1077,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1108,16 +1105,16 @@
         <v>53</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F1" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="25" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="30.75" thickBot="1">
+      <c r="G1" s="24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1">
       <c r="A2" s="17" t="s">
         <v>68</v>
       </c>
@@ -1128,7 +1125,7 @@
         <v>16730</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>69</v>
+        <v>156</v>
       </c>
       <c r="E2" s="18">
         <v>200</v>
@@ -1136,8 +1133,8 @@
       <c r="F2" s="18">
         <v>200</v>
       </c>
-      <c r="G2" s="24">
-        <v>404</v>
+      <c r="G2" s="18">
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30.75" thickBot="1">
@@ -1168,10 +1165,10 @@
         <v>57</v>
       </c>
       <c r="B4" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>70</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>71</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>58</v>
@@ -1220,7 +1217,7 @@
         <v>62</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E6" s="20">
         <v>401</v>
@@ -1239,7 +1236,7 @@
       <c r="B7" s="18"/>
       <c r="C7" s="18"/>
       <c r="D7" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E7" s="20">
         <v>405</v>
@@ -1256,13 +1253,13 @@
         <v>64</v>
       </c>
       <c r="B8" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="21" t="s">
-        <v>73</v>
-      </c>
       <c r="D8" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E8" s="22">
         <v>401</v>
@@ -1279,10 +1276,10 @@
         <v>65</v>
       </c>
       <c r="B9" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>101</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>102</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="23">
@@ -1304,31 +1301,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="26" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" style="26" customWidth="1"/>
-    <col min="3" max="3" width="26" style="26" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="26" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" style="26" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="26" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" style="26" customWidth="1"/>
-    <col min="8" max="8" width="28.42578125" style="26" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" style="26" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" style="26" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" style="26" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" style="26" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="26" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="26"/>
+    <col min="1" max="1" width="18.85546875" style="25" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" style="25" customWidth="1"/>
+    <col min="3" max="3" width="26" style="25" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="25" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="25" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="25" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" style="25" customWidth="1"/>
+    <col min="8" max="8" width="28.42578125" style="25" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" style="25" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" style="25" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" style="25" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" style="25" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" style="25" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="30.75" thickBot="1">
       <c r="A1" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>2</v>
@@ -1375,7 +1372,7 @@
         <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D2" s="3">
         <v>10</v>
@@ -1390,7 +1387,7 @@
         <v>16</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I2" s="3">
         <v>18</v>
@@ -1416,7 +1413,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D3" s="3">
         <v>10</v>
@@ -1431,7 +1428,7 @@
         <v>19</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I3" s="3">
         <v>18</v>
@@ -1449,52 +1446,52 @@
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="29" customFormat="1" ht="30.75" thickBot="1">
+    <row r="4" spans="1:13" s="28" customFormat="1" ht="30.75" thickBot="1">
       <c r="A4" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="D4" s="27">
+      <c r="D4" s="26">
         <v>10</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="26" t="s">
         <v>15</v>
       </c>
       <c r="F4" s="3">
         <v>16448</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="I4" s="27">
+      <c r="G4" s="26"/>
+      <c r="H4" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="I4" s="26">
         <v>18</v>
       </c>
-      <c r="J4" s="27" t="s">
+      <c r="J4" s="26" t="s">
         <v>15</v>
       </c>
       <c r="K4" s="3">
         <v>16448</v>
       </c>
-      <c r="L4" s="28">
+      <c r="L4" s="27">
         <v>201</v>
       </c>
-      <c r="M4" s="28">
+      <c r="M4" s="27">
         <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="30.75" thickBot="1">
       <c r="A5" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="3">
         <v>10</v>
@@ -1509,7 +1506,7 @@
         <v>16</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I5" s="3">
         <v>18</v>
@@ -1529,7 +1526,7 @@
     </row>
     <row r="6" spans="1:13" ht="30" thickBot="1">
       <c r="A6" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>14</v>
@@ -1560,7 +1557,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
@@ -1573,7 +1570,7 @@
         <v>16</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3" t="s">
@@ -1597,7 +1594,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D8" s="3">
         <v>10</v>
@@ -1610,7 +1607,7 @@
         <v>16</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I8" s="3">
         <v>18</v>
@@ -1634,7 +1631,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D9" s="3">
         <v>10</v>
@@ -1647,7 +1644,7 @@
         <v>16</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I9" s="3">
         <v>18</v>
@@ -1748,7 +1745,7 @@
       <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="26">
+      <c r="C12" s="25">
         <v>45678223789</v>
       </c>
       <c r="D12" s="3">
@@ -1763,7 +1760,7 @@
       <c r="G12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="26">
+      <c r="H12" s="25">
         <v>45678223789</v>
       </c>
       <c r="I12" s="3">
@@ -1790,7 +1787,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D13" s="3">
         <v>10</v>
@@ -1805,7 +1802,7 @@
         <v>16</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I13" s="3">
         <v>18</v>
@@ -1831,7 +1828,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D14" s="3">
         <v>0</v>
@@ -1846,7 +1843,7 @@
         <v>16</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I14" s="3">
         <v>0</v>
@@ -1872,7 +1869,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D15" s="3">
         <v>-10</v>
@@ -1887,7 +1884,7 @@
         <v>16</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I15" s="3">
         <v>-18</v>
@@ -1913,7 +1910,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D16" s="3">
         <v>10</v>
@@ -1928,7 +1925,7 @@
         <v>16</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I16" s="3">
         <v>18</v>
@@ -1954,7 +1951,7 @@
         <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D17" s="3">
         <v>10</v>
@@ -1969,7 +1966,7 @@
         <v>16</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I17" s="3">
         <v>18</v>
@@ -1995,7 +1992,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D18" s="3">
         <v>10</v>
@@ -2010,7 +2007,7 @@
         <v>16</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I18" s="3">
         <v>18</v>
@@ -2036,7 +2033,7 @@
         <v>14</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D19" s="3">
         <v>10</v>
@@ -2051,7 +2048,7 @@
         <v>16</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I19" s="3">
         <v>18</v>
@@ -2077,7 +2074,7 @@
         <v>14</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D20" s="3">
         <v>10</v>
@@ -2092,7 +2089,7 @@
         <v>16</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I20" s="3">
         <v>18</v>
@@ -2118,7 +2115,7 @@
         <v>14</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D21" s="3">
         <v>10</v>
@@ -2133,7 +2130,7 @@
         <v>16</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I21" s="3">
         <v>18</v>
@@ -2159,7 +2156,7 @@
         <v>14</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D22" s="3">
         <v>10</v>
@@ -2174,7 +2171,7 @@
         <v>16</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I22" s="3">
         <v>18</v>
@@ -2200,7 +2197,7 @@
         <v>14</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D23" s="3">
         <v>10</v>
@@ -2215,7 +2212,7 @@
         <v>16</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I23" s="3">
         <v>18</v>
@@ -2241,7 +2238,7 @@
         <v>44</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D24" s="3">
         <v>10</v>
@@ -2256,7 +2253,7 @@
         <v>44</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I24" s="3">
         <v>18</v>
@@ -2282,7 +2279,7 @@
         <v>2345678</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D25" s="3">
         <v>10</v>
@@ -2297,7 +2294,7 @@
         <v>2345678</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I25" s="3">
         <v>18</v>
@@ -2323,7 +2320,7 @@
         <v>47</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D26" s="3">
         <v>10</v>
@@ -2338,7 +2335,7 @@
         <v>48</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I26" s="3">
         <v>18</v>
@@ -2364,7 +2361,7 @@
         <v>14</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D27" s="3">
         <v>10</v>
@@ -2379,7 +2376,7 @@
         <v>16</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I27" s="3">
         <v>18</v>
@@ -2421,115 +2418,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="61.5" thickTop="1" thickBot="1">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="E1" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="R1" s="30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="45.75" thickBot="1">
+      <c r="A2" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="E1" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="F1" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="G1" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="H1" s="30" t="s">
+      <c r="B2" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="I1" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="P1" s="31" t="s">
+      <c r="F2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="34">
+        <v>201</v>
+      </c>
+      <c r="J2" s="34">
+        <v>200</v>
+      </c>
+      <c r="K2" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="31">
         <v>10</v>
       </c>
-      <c r="Q1" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="R1" s="31" t="s">
+      <c r="M2" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="O2" s="31">
+        <v>15</v>
+      </c>
+      <c r="P2" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" s="31" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="45.75" thickBot="1">
-      <c r="A2" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="35">
-        <v>201</v>
-      </c>
-      <c r="J2" s="35">
-        <v>200</v>
-      </c>
-      <c r="K2" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="32">
-        <v>10</v>
-      </c>
-      <c r="M2" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="O2" s="32">
-        <v>15</v>
-      </c>
-      <c r="P2" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q2" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="R2" s="32" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2549,128 +2546,128 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:21" ht="60.75" thickBot="1">
-      <c r="A1" s="39" t="s">
-        <v>79</v>
+      <c r="A1" s="38" t="s">
+        <v>78</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="Q1" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="R1" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="T1" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="U1" s="35" t="s">
         <v>125</v>
       </c>
-      <c r="U1" s="36" t="s">
-        <v>126</v>
-      </c>
     </row>
     <row r="2" spans="1:21" ht="75.75" thickBot="1">
-      <c r="A2" s="40" t="s">
-        <v>139</v>
+      <c r="A2" s="39" t="s">
+        <v>138</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="I2" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="37" t="s">
         <v>143</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I2" s="37" t="s">
-        <v>132</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="O2" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="P2" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q2" s="38" t="s">
-        <v>144</v>
       </c>
       <c r="R2" s="10"/>
       <c r="S2" s="10" t="s">
         <v>15</v>
       </c>
       <c r="T2" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="U2" s="35">
+        <v>137</v>
+      </c>
+      <c r="U2" s="34">
         <v>201</v>
       </c>
     </row>
@@ -2694,118 +2691,118 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:21" ht="60.75" thickBot="1">
-      <c r="A1" s="39" t="s">
-        <v>79</v>
+      <c r="A1" s="38" t="s">
+        <v>78</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="Q1" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="R1" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="T1" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="U1" s="35" t="s">
         <v>125</v>
       </c>
-      <c r="U1" s="36" t="s">
-        <v>126</v>
-      </c>
     </row>
     <row r="2" spans="1:21" ht="75.75" thickBot="1">
-      <c r="A2" s="40" t="s">
-        <v>139</v>
+      <c r="A2" s="39" t="s">
+        <v>138</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="I2" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="L2" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I2" s="37" t="s">
-        <v>132</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>141</v>
-      </c>
       <c r="M2" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N2" s="10"/>
       <c r="O2" s="10"/>
       <c r="P2" s="10"/>
-      <c r="Q2" s="38" t="s">
-        <v>146</v>
+      <c r="Q2" s="37" t="s">
+        <v>145</v>
       </c>
       <c r="R2" s="10"/>
       <c r="S2" s="10"/>
       <c r="T2" s="10"/>
-      <c r="U2" s="35">
+      <c r="U2" s="34">
         <v>200</v>
       </c>
     </row>
@@ -2829,124 +2826,124 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:21" ht="60.75" thickBot="1">
-      <c r="A1" s="39" t="s">
-        <v>79</v>
+      <c r="A1" s="38" t="s">
+        <v>78</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q1" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="R1" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="S1" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="Q1" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="R1" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="S1" s="10" t="s">
+      <c r="T1" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="U1" s="35" t="s">
         <v>125</v>
       </c>
-      <c r="U1" s="36" t="s">
-        <v>126</v>
-      </c>
     </row>
     <row r="2" spans="1:21" ht="75.75" thickBot="1">
-      <c r="A2" s="40" t="s">
-        <v>139</v>
+      <c r="A2" s="39" t="s">
+        <v>138</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="I2" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="L2" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I2" s="37" t="s">
-        <v>132</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>141</v>
-      </c>
       <c r="M2" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O2" s="10"/>
       <c r="P2" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Q2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="38" t="s">
-        <v>148</v>
+      <c r="R2" s="37" t="s">
+        <v>147</v>
       </c>
       <c r="S2" s="10"/>
       <c r="T2" s="10"/>
-      <c r="U2" s="35">
+      <c r="U2" s="34">
         <v>200</v>
       </c>
     </row>
@@ -2963,61 +2960,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8" ht="60.75" thickBot="1">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="42" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="42" t="s">
         <v>149</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="F1" s="42" t="s">
         <v>150</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="G1" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="43" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="45.75" thickBot="1">
+      <c r="A2" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="32">
+        <v>16652</v>
+      </c>
+      <c r="C2" s="32">
+        <v>8608</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="32" t="s">
         <v>151</v>
       </c>
-      <c r="G1" s="43" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="44" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="45.75" thickBot="1">
-      <c r="A2" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="33">
-        <v>16652</v>
-      </c>
-      <c r="C2" s="33">
-        <v>8608</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="33" t="s">
-        <v>152</v>
-      </c>
-      <c r="F2" s="33" t="s">
-        <v>138</v>
-      </c>
-      <c r="G2" s="34">
+      <c r="F2" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="G2" s="33">
         <v>200</v>
       </c>
-      <c r="H2" s="34">
+      <c r="H2" s="33">
         <v>200</v>
       </c>
     </row>
@@ -3037,37 +3034,37 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6" ht="45.75" thickBot="1">
-      <c r="A1" s="45" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" s="46" t="s">
+      <c r="A1" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="45" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="45" t="s">
         <v>153</v>
       </c>
-      <c r="D1" s="46" t="s">
-        <v>107</v>
-      </c>
-      <c r="E1" s="46" t="s">
+      <c r="F1" s="46" t="s">
         <v>154</v>
       </c>
-      <c r="F1" s="47" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A2" s="47" t="s">
         <v>155</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A2" s="48" t="s">
-        <v>156</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
       <c r="F2" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working ETE All Modules
</commit_message>
<xml_diff>
--- a/Team17_APINinjas_LMSHack/src/test/resources/LMSAPINinjaTestData.xlsx
+++ b/Team17_APINinjas_LMSHack/src/test/resources/LMSAPINinjaTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="22950" windowHeight="9360" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="22950" windowHeight="9360" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="GetDeleteTestData-BatchJyo" sheetId="5" r:id="rId1"/>
@@ -449,21 +449,12 @@
     <t>R01</t>
   </si>
   <si>
-    <t>4156169xxx</t>
-  </si>
-  <si>
     <t>APIemailxxx@gmail.com</t>
   </si>
   <si>
-    <t>4356169xxx</t>
-  </si>
-  <si>
     <t>Ninjasemailxxx@gmail.com</t>
   </si>
   <si>
-    <t>4456169xxx</t>
-  </si>
-  <si>
     <t>APINinjasmyemailxxx@gmail.com</t>
   </si>
   <si>
@@ -492,6 +483,15 @@
   </si>
   <si>
     <t>March24-Api Ninjas</t>
+  </si>
+  <si>
+    <t>4152169xxx</t>
+  </si>
+  <si>
+    <t>4352169xxx</t>
+  </si>
+  <si>
+    <t>4452169xxx</t>
   </si>
 </sst>
 </file>
@@ -1125,7 +1125,7 @@
         <v>16730</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E2" s="18">
         <v>200</v>
@@ -1301,7 +1301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -2616,7 +2616,7 @@
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>126</v>
@@ -2658,7 +2658,7 @@
         <v>15</v>
       </c>
       <c r="Q2" s="37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="R2" s="10"/>
       <c r="S2" s="10" t="s">
@@ -2685,7 +2685,7 @@
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2761,7 +2761,7 @@
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>126</v>
@@ -2797,7 +2797,7 @@
       <c r="O2" s="10"/>
       <c r="P2" s="10"/>
       <c r="Q2" s="37" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="R2" s="10"/>
       <c r="S2" s="10"/>
@@ -2819,8 +2819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2896,7 +2896,7 @@
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>126</v>
@@ -2939,7 +2939,7 @@
         <v>15</v>
       </c>
       <c r="R2" s="37" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="S2" s="10"/>
       <c r="T2" s="10"/>
@@ -2977,13 +2977,13 @@
         <v>51</v>
       </c>
       <c r="D1" s="42" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E1" s="42" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F1" s="42" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G1" s="42" t="s">
         <v>12</v>
@@ -3006,7 +3006,7 @@
         <v>15</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F2" s="32" t="s">
         <v>137</v>
@@ -3041,21 +3041,21 @@
         <v>6</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>106</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F1" s="46" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1">
       <c r="A2" s="47" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10" t="s">

</xml_diff>

<commit_message>
ETE Working Added User Negatives
</commit_message>
<xml_diff>
--- a/Team17_APINinjas_LMSHack/src/test/resources/LMSAPINinjaTestData.xlsx
+++ b/Team17_APINinjas_LMSHack/src/test/resources/LMSAPINinjaTestData.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Java\Team17_APINinjas\Team17_APINinjas_LMSHack\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA0431E-0E72-4F19-A828-CB67CCA0F39F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="11505" firstSheet="5" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="PutLoginStatusNegative" sheetId="17" r:id="rId1"/>
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="198">
   <si>
     <t>TestCaseNumbers</t>
   </si>
@@ -462,15 +456,9 @@
     <t>R01</t>
   </si>
   <si>
-    <t>4156169xxx</t>
-  </si>
-  <si>
     <t>4356169xxx</t>
   </si>
   <si>
-    <t>4456169xxx</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -555,15 +543,9 @@
     <t>APINinjasmyemail9999@gmail.com</t>
   </si>
   <si>
-    <t>APINinjamyemailxxx@gmail.com</t>
-  </si>
-  <si>
     <t>Ninjaemailxxx@gmail.com</t>
   </si>
   <si>
-    <t>APINinjaemailxxx@gmail.com</t>
-  </si>
-  <si>
     <t>U234111</t>
   </si>
   <si>
@@ -619,13 +601,31 @@
   </si>
   <si>
     <t>PSTXX</t>
+  </si>
+  <si>
+    <t>4156168xxx</t>
+  </si>
+  <si>
+    <t>APINinjAemailxxx@gmail.com</t>
+  </si>
+  <si>
+    <t>4356168xxx</t>
+  </si>
+  <si>
+    <t>ninjaemailxxx@gmail.com</t>
+  </si>
+  <si>
+    <t>ApINinjamyemailxxx@gmail.com</t>
+  </si>
+  <si>
+    <t>4456168xxx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -939,9 +939,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -979,7 +979,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1013,7 +1013,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1048,10 +1047,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1224,23 +1222,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C0A49E0-6D6D-48B5-9785-2AC7B177B678}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.6328125" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" customWidth="1"/>
-    <col min="7" max="7" width="32.54296875" customWidth="1"/>
+    <col min="1" max="1" width="35.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="32.5703125" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="30.75" thickBot="1">
       <c r="A1" s="39" t="s">
         <v>79</v>
       </c>
@@ -1268,12 +1266,12 @@
       <c r="I1" s="52"/>
       <c r="J1" s="52"/>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1">
       <c r="A2" s="40" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>105</v>
@@ -1286,18 +1284,18 @@
         <v>15</v>
       </c>
       <c r="G2" s="38" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H2" s="49" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="30.75" thickBot="1">
       <c r="A3" s="40" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>105</v>
@@ -1307,21 +1305,21 @@
         <v>142</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G3" s="38" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H3" s="49" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="30.75" thickBot="1">
       <c r="A4" s="40" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>105</v>
@@ -1334,42 +1332,42 @@
         <v>15</v>
       </c>
       <c r="G4" s="38" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H4" s="49" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1">
       <c r="A5" s="40" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>105</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="38" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H5" s="49" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1">
       <c r="A6" s="53" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -1380,40 +1378,40 @@
         <v>15</v>
       </c>
       <c r="G6" s="38" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H6" s="49" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{B663B328-14FF-4DF7-961C-312E694C364C}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{FA816064-9007-4740-87B2-509999B081DE}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{7494CB9F-03F4-4DCB-8C17-4D2DC83878AB}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{2FF65A17-DF5C-4C9C-99AB-198EA76D4F9E}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{7DFD70D4-F422-478F-A846-1748939EBCF7}"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="G6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C869987-B931-453F-B22C-FCE8289E4B68}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="32.6328125" customWidth="1"/>
-    <col min="14" max="14" width="23.54296875" customWidth="1"/>
-    <col min="15" max="15" width="20.08984375" customWidth="1"/>
+    <col min="1" max="1" width="32.5703125" customWidth="1"/>
+    <col min="14" max="14" width="23.5703125" customWidth="1"/>
+    <col min="15" max="15" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" ht="30.75" thickBot="1">
       <c r="A1" s="39" t="s">
         <v>79</v>
       </c>
@@ -1460,15 +1458,15 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="73" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" ht="75.75" thickBot="1">
       <c r="A2" s="40" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>127</v>
@@ -1501,21 +1499,21 @@
         <v>136</v>
       </c>
       <c r="N2" s="38" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="O2" s="49" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="73" thickBot="1" x14ac:dyDescent="0.4">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="75.75" thickBot="1">
       <c r="A3" s="40" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>127</v>
@@ -1524,7 +1522,7 @@
         <v>140</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>130</v>
@@ -1548,34 +1546,34 @@
         <v>136</v>
       </c>
       <c r="N3" s="38" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="O3" s="49" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{5E8E8A38-A801-4B5A-BEEA-71DFDFC91883}"/>
-    <hyperlink ref="N2" r:id="rId2" xr:uid="{163E956C-A713-4F6B-8B33-E1A06D62B693}"/>
-    <hyperlink ref="I3" r:id="rId3" xr:uid="{FC1F64FF-340E-4724-B0D3-A76F91F4D6E2}"/>
-    <hyperlink ref="N3" r:id="rId4" xr:uid="{36D84669-5665-4E79-918C-0DA371968D14}"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="N2" r:id="rId2"/>
+    <hyperlink ref="I3" r:id="rId3"/>
+    <hyperlink ref="N3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="57" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="60.75" thickBot="1">
       <c r="A1" s="42" t="s">
         <v>1</v>
       </c>
@@ -1586,13 +1584,13 @@
         <v>51</v>
       </c>
       <c r="D1" s="43" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" s="43" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" s="43" t="s">
         <v>146</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>147</v>
-      </c>
-      <c r="F1" s="43" t="s">
-        <v>148</v>
       </c>
       <c r="G1" s="43" t="s">
         <v>12</v>
@@ -1601,7 +1599,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" ht="45.75" thickBot="1">
       <c r="A2" s="41" t="s">
         <v>50</v>
       </c>
@@ -1615,7 +1613,7 @@
         <v>15</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F2" s="33" t="s">
         <v>138</v>
@@ -1633,20 +1631,20 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.7265625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="7" max="7" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="32.25" thickBot="1">
       <c r="A1" s="45" t="s">
         <v>79</v>
       </c>
@@ -1654,24 +1652,24 @@
         <v>6</v>
       </c>
       <c r="C1" s="46" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D1" s="46" t="s">
         <v>107</v>
       </c>
       <c r="E1" s="46" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F1" s="47" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G1" s="36" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="30.75" thickBot="1">
       <c r="A2" s="45" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10" t="s">
@@ -1683,7 +1681,7 @@
         <v>105</v>
       </c>
       <c r="G2" s="49" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -1692,29 +1690,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D7256EE-5B91-40B5-90F2-95BE40CC9D82}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.36328125" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" customWidth="1"/>
-    <col min="4" max="4" width="12.26953125" customWidth="1"/>
-    <col min="5" max="5" width="12.90625" customWidth="1"/>
-    <col min="9" max="9" width="12.36328125" customWidth="1"/>
-    <col min="12" max="12" width="12.453125" customWidth="1"/>
-    <col min="14" max="14" width="15.26953125" customWidth="1"/>
-    <col min="15" max="15" width="14.54296875" customWidth="1"/>
-    <col min="17" max="17" width="22.90625" customWidth="1"/>
-    <col min="19" max="19" width="12.90625" customWidth="1"/>
-    <col min="21" max="21" width="20.36328125" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" customWidth="1"/>
+    <col min="17" max="17" width="22.85546875" customWidth="1"/>
+    <col min="19" max="19" width="12.85546875" customWidth="1"/>
+    <col min="21" max="21" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:21" ht="45.75" thickBot="1">
       <c r="A1" s="39" t="s">
         <v>79</v>
       </c>
@@ -1779,22 +1777,22 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:21" ht="60.75" thickBot="1">
       <c r="A2" s="50" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="48" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>128</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>130</v>
@@ -1827,7 +1825,7 @@
         <v>15</v>
       </c>
       <c r="Q2" s="38" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="R2" s="10"/>
       <c r="S2" s="10" t="s">
@@ -1837,19 +1835,19 @@
         <v>138</v>
       </c>
       <c r="U2" s="49" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="60.75" thickBot="1">
       <c r="A3" s="50" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="48" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>140</v>
@@ -1888,7 +1886,7 @@
         <v>15</v>
       </c>
       <c r="Q3" s="38" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="R3" s="10"/>
       <c r="S3" s="10" t="s">
@@ -1898,23 +1896,23 @@
         <v>106</v>
       </c>
       <c r="U3" s="49" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="60.75" thickBot="1">
       <c r="A4" s="50" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="48" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10" t="s">
         <v>128</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>130</v>
@@ -1947,7 +1945,7 @@
         <v>15</v>
       </c>
       <c r="Q4" s="38" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="R4" s="10"/>
       <c r="S4" s="10" t="s">
@@ -1957,25 +1955,25 @@
         <v>138</v>
       </c>
       <c r="U4" s="49" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="60.75" thickBot="1">
       <c r="A5" s="50" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="48" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>128</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>130</v>
@@ -2008,7 +2006,7 @@
         <v>15</v>
       </c>
       <c r="Q5" s="38" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="R5" s="10"/>
       <c r="S5" s="10" t="s">
@@ -2018,44 +2016,44 @@
         <v>138</v>
       </c>
       <c r="U5" s="49" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{12625F93-3309-4FE6-ACD3-CD22D330B13E}"/>
-    <hyperlink ref="Q2" r:id="rId2" xr:uid="{23A1E0F8-D7FA-4B65-8F0C-851B866E6916}"/>
-    <hyperlink ref="I3" r:id="rId3" xr:uid="{AFF521B5-436D-4F70-9CE4-673811BEA78E}"/>
-    <hyperlink ref="Q3" r:id="rId4" xr:uid="{7451DF1E-2535-40AB-82C8-B5DF1D9A47A0}"/>
-    <hyperlink ref="I4" r:id="rId5" xr:uid="{EE39C246-12EC-4851-B514-1F47CC0B3AD5}"/>
-    <hyperlink ref="Q4" r:id="rId6" xr:uid="{B18904D5-4513-410A-9B43-42B0A28DCBF4}"/>
-    <hyperlink ref="I5" r:id="rId7" xr:uid="{1CF3A76F-8D40-491F-B751-8176D9ECDA66}"/>
-    <hyperlink ref="Q5" r:id="rId8" xr:uid="{98BC6695-548E-47EE-82A8-CF497E46DD7E}"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="Q2" r:id="rId2"/>
+    <hyperlink ref="I3" r:id="rId3"/>
+    <hyperlink ref="Q3" r:id="rId4"/>
+    <hyperlink ref="I4" r:id="rId5"/>
+    <hyperlink ref="Q4" r:id="rId6"/>
+    <hyperlink ref="I5" r:id="rId7"/>
+    <hyperlink ref="Q5" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.54296875" customWidth="1"/>
-    <col min="2" max="2" width="19.54296875" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" customWidth="1"/>
-    <col min="4" max="4" width="18.81640625" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="21.7265625" customWidth="1"/>
-    <col min="7" max="7" width="17.54296875" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="30.75" thickBot="1">
       <c r="A1" s="15" t="s">
         <v>67</v>
       </c>
@@ -2078,7 +2076,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="30.75" thickBot="1">
       <c r="A2" s="17" t="s">
         <v>68</v>
       </c>
@@ -2101,7 +2099,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="30.75" thickBot="1">
       <c r="A3" s="17" t="s">
         <v>55</v>
       </c>
@@ -2124,7 +2122,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="43.5" thickBot="1">
       <c r="A4" s="19" t="s">
         <v>57</v>
       </c>
@@ -2147,7 +2145,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="43.5" thickBot="1">
       <c r="A5" s="19" t="s">
         <v>59</v>
       </c>
@@ -2170,7 +2168,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="86.25" thickBot="1">
       <c r="A6" s="19" t="s">
         <v>61</v>
       </c>
@@ -2193,7 +2191,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="57.75" thickBot="1">
       <c r="A7" s="19" t="s">
         <v>63</v>
       </c>
@@ -2212,7 +2210,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="86.25" thickBot="1">
       <c r="A8" s="19" t="s">
         <v>64</v>
       </c>
@@ -2235,7 +2233,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="43.5" thickBot="1">
       <c r="A9" s="22" t="s">
         <v>65</v>
       </c>
@@ -2262,32 +2260,32 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.81640625" style="26" customWidth="1"/>
-    <col min="2" max="2" width="23.81640625" style="26" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" style="26" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" style="26" customWidth="1"/>
     <col min="3" max="3" width="26" style="26" customWidth="1"/>
-    <col min="4" max="4" width="15.453125" style="26" customWidth="1"/>
-    <col min="5" max="5" width="16.7265625" style="26" customWidth="1"/>
-    <col min="6" max="6" width="19.1796875" style="26" customWidth="1"/>
-    <col min="7" max="7" width="18.1796875" style="26" customWidth="1"/>
-    <col min="8" max="8" width="28.453125" style="26" customWidth="1"/>
-    <col min="9" max="9" width="12.81640625" style="26" customWidth="1"/>
-    <col min="10" max="10" width="14.81640625" style="26" customWidth="1"/>
-    <col min="11" max="11" width="15.453125" style="26" customWidth="1"/>
-    <col min="12" max="12" width="16.453125" style="26" customWidth="1"/>
-    <col min="13" max="13" width="19.453125" style="26" customWidth="1"/>
-    <col min="14" max="16384" width="9.1796875" style="26"/>
+    <col min="4" max="4" width="15.42578125" style="26" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="26" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="26" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" style="26" customWidth="1"/>
+    <col min="8" max="8" width="28.42578125" style="26" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" style="26" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" style="26" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" style="26" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" style="26" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" style="26" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="30.75" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>79</v>
       </c>
@@ -2328,7 +2326,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="56.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" ht="72" thickBot="1">
       <c r="A2" s="9" t="s">
         <v>17</v>
       </c>
@@ -2369,7 +2367,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" ht="86.25" thickBot="1">
       <c r="A3" s="9" t="s">
         <v>18</v>
       </c>
@@ -2410,7 +2408,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="29" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" s="29" customFormat="1" ht="30.75" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>85</v>
       </c>
@@ -2447,7 +2445,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" ht="30.75" thickBot="1">
       <c r="A5" s="1" t="s">
         <v>80</v>
       </c>
@@ -2488,7 +2486,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" ht="30" thickBot="1">
       <c r="A6" s="12" t="s">
         <v>84</v>
       </c>
@@ -2513,7 +2511,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13" ht="30.75" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>27</v>
       </c>
@@ -2550,7 +2548,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" ht="30.75" thickBot="1">
       <c r="A8" s="9" t="s">
         <v>20</v>
       </c>
@@ -2587,7 +2585,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:13" ht="30.75" thickBot="1">
       <c r="A9" s="9" t="s">
         <v>28</v>
       </c>
@@ -2624,7 +2622,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" ht="43.5" thickBot="1">
       <c r="A10" s="9" t="s">
         <v>21</v>
       </c>
@@ -2665,7 +2663,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:13" ht="15.75" thickBot="1">
       <c r="A11" s="9" t="s">
         <v>23</v>
       </c>
@@ -2702,7 +2700,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:13" ht="43.5" thickBot="1">
       <c r="A12" s="9" t="s">
         <v>24</v>
       </c>
@@ -2743,7 +2741,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:13" ht="43.5" thickBot="1">
       <c r="A13" s="9" t="s">
         <v>25</v>
       </c>
@@ -2784,7 +2782,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:13" ht="30.75" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>29</v>
       </c>
@@ -2825,7 +2823,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:13" ht="43.5" thickBot="1">
       <c r="A15" s="9" t="s">
         <v>30</v>
       </c>
@@ -2866,7 +2864,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="56.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:13" ht="57.75" thickBot="1">
       <c r="A16" s="9" t="s">
         <v>31</v>
       </c>
@@ -2907,7 +2905,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:13" ht="57.75" thickBot="1">
       <c r="A17" s="9" t="s">
         <v>33</v>
       </c>
@@ -2948,7 +2946,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:13" ht="57.75" thickBot="1">
       <c r="A18" s="9" t="s">
         <v>35</v>
       </c>
@@ -2989,7 +2987,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:13" ht="43.5" thickBot="1">
       <c r="A19" s="9" t="s">
         <v>37</v>
       </c>
@@ -3030,7 +3028,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:13" ht="43.5" thickBot="1">
       <c r="A20" s="9" t="s">
         <v>38</v>
       </c>
@@ -3071,7 +3069,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:13" ht="30.75" thickBot="1">
       <c r="A21" s="9" t="s">
         <v>40</v>
       </c>
@@ -3112,7 +3110,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:13" ht="30.75" thickBot="1">
       <c r="A22" s="9" t="s">
         <v>41</v>
       </c>
@@ -3153,7 +3151,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:13" ht="43.5" thickBot="1">
       <c r="A23" s="9" t="s">
         <v>42</v>
       </c>
@@ -3194,7 +3192,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="56.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:13" ht="57.75" thickBot="1">
       <c r="A24" s="9" t="s">
         <v>43</v>
       </c>
@@ -3235,7 +3233,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:13" ht="43.5" thickBot="1">
       <c r="A25" s="9" t="s">
         <v>45</v>
       </c>
@@ -3276,7 +3274,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:13" ht="57.75" thickBot="1">
       <c r="A26" s="9" t="s">
         <v>46</v>
       </c>
@@ -3317,7 +3315,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:13" ht="30.75" thickBot="1">
       <c r="A27" s="9" t="s">
         <v>49</v>
       </c>
@@ -3364,24 +3362,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" customWidth="1"/>
-    <col min="2" max="2" width="18.453125" customWidth="1"/>
-    <col min="3" max="3" width="18.54296875" customWidth="1"/>
-    <col min="4" max="4" width="18.1796875" customWidth="1"/>
-    <col min="5" max="5" width="19.453125" customWidth="1"/>
-    <col min="10" max="10" width="15.26953125" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="57.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" ht="61.5" thickTop="1" thickBot="1">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -3437,7 +3435,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:18" ht="45.75" thickBot="1">
       <c r="A2" s="34" t="s">
         <v>98</v>
       </c>
@@ -3500,16 +3498,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:21" ht="60.75" thickBot="1">
       <c r="A1" s="39" t="s">
         <v>79</v>
       </c>
@@ -3574,13 +3572,13 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="73" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:21" ht="75.75" thickBot="1">
       <c r="A2" s="40" t="s">
         <v>139</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10" t="s">
-        <v>143</v>
+        <v>192</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>127</v>
@@ -3622,7 +3620,7 @@
         <v>15</v>
       </c>
       <c r="Q2" s="38" t="s">
-        <v>176</v>
+        <v>193</v>
       </c>
       <c r="R2" s="10"/>
       <c r="S2" s="10" t="s">
@@ -3637,24 +3635,24 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="Q2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="Q2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:21" ht="60.75" thickBot="1">
       <c r="A1" s="39" t="s">
         <v>79</v>
       </c>
@@ -3719,13 +3717,13 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="73" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:21" ht="75.75" thickBot="1">
       <c r="A2" s="40" t="s">
         <v>139</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10" t="s">
-        <v>144</v>
+        <v>194</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>127</v>
@@ -3761,7 +3759,7 @@
       <c r="O2" s="10"/>
       <c r="P2" s="10"/>
       <c r="Q2" s="38" t="s">
-        <v>175</v>
+        <v>195</v>
       </c>
       <c r="R2" s="10"/>
       <c r="S2" s="10"/>
@@ -3772,24 +3770,24 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="Q2" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="Q2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:21" ht="60.75" thickBot="1">
       <c r="A1" s="39" t="s">
         <v>79</v>
       </c>
@@ -3854,13 +3852,13 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="73" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:21" ht="75.75" thickBot="1">
       <c r="A2" s="40" t="s">
         <v>139</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10" t="s">
-        <v>145</v>
+        <v>197</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>127</v>
@@ -3903,7 +3901,7 @@
         <v>15</v>
       </c>
       <c r="R2" s="38" t="s">
-        <v>174</v>
+        <v>196</v>
       </c>
       <c r="S2" s="10"/>
       <c r="T2" s="10"/>
@@ -3913,29 +3911,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="R2" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="R2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{592C7846-7F54-46C4-9F7C-BE63FE12C252}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.81640625" customWidth="1"/>
-    <col min="6" max="6" width="25.90625" customWidth="1"/>
-    <col min="7" max="7" width="21.54296875" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="32.25" thickBot="1">
       <c r="A1" s="45" t="s">
         <v>79</v>
       </c>
@@ -3943,111 +3941,111 @@
         <v>6</v>
       </c>
       <c r="C1" s="46" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D1" s="46" t="s">
         <v>107</v>
       </c>
       <c r="E1" s="46" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F1" s="47" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G1" s="36" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="15.75" thickBot="1">
       <c r="A2" s="51" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>138</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E2" s="48" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>105</v>
       </c>
       <c r="G2" s="49" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30.75" thickBot="1">
       <c r="A3" s="45" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>138</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E3" s="48" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>105</v>
       </c>
       <c r="G3" s="49" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30.75" thickBot="1">
       <c r="A4" s="45" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B4" s="48" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>138</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E4" s="48" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>105</v>
       </c>
       <c r="G4" s="49" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30.75" thickBot="1">
       <c r="A5" s="45" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B5" s="48" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>138</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E5" s="48" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G5" s="49" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>